<commit_message>
added arcgis pro toolbox
</commit_message>
<xml_diff>
--- a/ICBC Rare Plant Fields.xlsx
+++ b/ICBC Rare Plant Fields.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIS\Projects\CHIS_RarePlants\rare-plants-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C083F69-8033-4DE7-BC93-59F87EE9EE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4007C6-F17C-48F0-981F-30D896EBFF2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,7 +423,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="36">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -618,6 +618,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF828B3"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -782,7 +788,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -792,6 +798,7 @@
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -839,6 +846,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF828B3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1150,7 +1162,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19:C32"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1507,7 +1519,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="9" t="s">
         <v>2</v>
       </c>
       <c r="B18" s="7" t="s">
@@ -1598,9 +1610,7 @@
       <c r="E22" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F22" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
@@ -1640,9 +1650,7 @@
       <c r="E24" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F24" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="F24" s="2"/>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
@@ -1682,9 +1690,7 @@
       <c r="E26" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F26" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="F26" s="2"/>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
@@ -1724,9 +1730,7 @@
       <c r="E28" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F28" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
@@ -1766,9 +1770,7 @@
       <c r="E30" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F30" s="2" t="b">
-        <v>0</v>
-      </c>
+      <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
@@ -1818,6 +1820,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002DD05BDEB67CCF49B1F62098075BD6BD" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c5ac96ff964cb127ddd2f025ea46fed1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ac1b8598-25a1-44b8-ad80-08c7b9b82e00" xmlns:ns4="91219154-ba08-4e37-8c3a-3f23ee0bbe1d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfb23bbfd9138cb2a517b19d89bf396f" ns3:_="" ns4:_="">
     <xsd:import namespace="ac1b8598-25a1-44b8-ad80-08c7b9b82e00"/>
@@ -2046,22 +2063,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{612725A2-A8FA-42C5-BACD-1CC770732C52}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="ac1b8598-25a1-44b8-ad80-08c7b9b82e00"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="91219154-ba08-4e37-8c3a-3f23ee0bbe1d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB43B128-AF66-4030-9A5B-9D67D87544CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25692AF8-A630-45EB-A690-3276AECE036E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2078,29 +2105,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB43B128-AF66-4030-9A5B-9D67D87544CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{612725A2-A8FA-42C5-BACD-1CC770732C52}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="ac1b8598-25a1-44b8-ad80-08c7b9b82e00"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="91219154-ba08-4e37-8c3a-3f23ee0bbe1d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
spatial reference, fixed short integer
</commit_message>
<xml_diff>
--- a/ICBC Rare Plant Fields.xlsx
+++ b/ICBC Rare Plant Fields.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIS\Projects\CHIS_RarePlants\rare-plants-tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981EE54F-864E-48AF-9E3E-2848964A22DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4AB91D-AEB0-42D5-A043-25D73D631892}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57490" yWindow="-10810" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NewFieldsAutomated" sheetId="13" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="89">
   <si>
     <t>Taxon</t>
   </si>
@@ -28,9 +28,6 @@
     <t>Observers</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t>Domain</t>
   </si>
   <si>
@@ -281,6 +278,15 @@
   </si>
   <si>
     <t>Date</t>
+  </si>
+  <si>
+    <t>Survey_Year</t>
+  </si>
+  <si>
+    <t>Survey Year</t>
+  </si>
+  <si>
+    <t>Data Resolution</t>
   </si>
 </sst>
 </file>
@@ -1162,7 +1168,7 @@
   <dimension ref="A1:H32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1177,42 +1183,42 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C2" s="3">
         <v>255</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1220,19 +1226,19 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C3" s="3">
+        <v>255</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>72</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="3">
-        <v>255</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>73</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
@@ -1240,17 +1246,19 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C4" s="3">
+        <v>255</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C4" s="3">
-        <v>255</v>
-      </c>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2" t="s">
-        <v>78</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
@@ -1258,19 +1266,19 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C5" s="3">
+        <v>255</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C5" s="3">
-        <v>255</v>
-      </c>
-      <c r="D5" s="3" t="s">
+      <c r="E5" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -1281,109 +1289,109 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="3">
         <v>255</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F6" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C7" s="3">
         <v>255</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" s="2"/>
       <c r="F7" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C8" s="3">
         <v>255</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="3">
+        <v>255</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="C9" s="3">
-        <v>255</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>35</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2" t="b">
         <v>1</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C10" s="3">
         <v>255</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -1392,16 +1400,16 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C11" s="3">
         <v>255</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -1410,16 +1418,16 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C12" s="3">
         <v>255</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
@@ -1428,54 +1436,54 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C13" s="3">
         <v>255</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C14" s="3">
         <v>255</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="b">
@@ -1486,14 +1494,14 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
@@ -1502,32 +1510,32 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>2</v>
+        <v>86</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="1" t="s">
-        <v>2</v>
+        <v>87</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
@@ -1536,16 +1544,16 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C19" s="7">
         <v>255</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
@@ -1554,19 +1562,19 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C20" s="7">
         <v>255</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F20" s="2" t="b">
         <v>1</v>
@@ -1576,19 +1584,19 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C21" s="7">
         <v>255</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F21" s="2"/>
       <c r="G21" s="2"/>
@@ -1596,19 +1604,19 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C22" s="7">
         <v>255</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
@@ -1616,19 +1624,19 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C23" s="7">
         <v>255</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F23" s="2"/>
       <c r="G23" s="2"/>
@@ -1636,19 +1644,19 @@
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" s="7">
         <v>255</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F24" s="2"/>
       <c r="G24" s="2"/>
@@ -1656,19 +1664,19 @@
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C25" s="7">
         <v>255</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F25" s="2"/>
       <c r="G25" s="2"/>
@@ -1676,19 +1684,19 @@
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C26" s="7">
         <v>255</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F26" s="2"/>
       <c r="G26" s="2"/>
@@ -1696,19 +1704,19 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C27" s="7">
         <v>255</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
@@ -1716,19 +1724,19 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C28" s="7">
         <v>255</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
@@ -1736,19 +1744,19 @@
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C29" s="7">
         <v>255</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
@@ -1756,19 +1764,19 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C30" s="7">
         <v>255</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
@@ -1776,19 +1784,19 @@
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C31" s="7">
         <v>255</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
@@ -1799,19 +1807,19 @@
         <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C32" s="7">
         <v>255</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -1820,6 +1828,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002DD05BDEB67CCF49B1F62098075BD6BD" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c5ac96ff964cb127ddd2f025ea46fed1">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="ac1b8598-25a1-44b8-ad80-08c7b9b82e00" xmlns:ns4="91219154-ba08-4e37-8c3a-3f23ee0bbe1d" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dfb23bbfd9138cb2a517b19d89bf396f" ns3:_="" ns4:_="">
     <xsd:import namespace="ac1b8598-25a1-44b8-ad80-08c7b9b82e00"/>
@@ -2048,22 +2071,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{612725A2-A8FA-42C5-BACD-1CC770732C52}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="ac1b8598-25a1-44b8-ad80-08c7b9b82e00"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="91219154-ba08-4e37-8c3a-3f23ee0bbe1d"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB43B128-AF66-4030-9A5B-9D67D87544CA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{25692AF8-A630-45EB-A690-3276AECE036E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2080,29 +2113,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AB43B128-AF66-4030-9A5B-9D67D87544CA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{612725A2-A8FA-42C5-BACD-1CC770732C52}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="ac1b8598-25a1-44b8-ad80-08c7b9b82e00"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="91219154-ba08-4e37-8c3a-3f23ee0bbe1d"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>